<commit_message>
modify tables count percentage
</commit_message>
<xml_diff>
--- a/KMP_fault_seeded.xlsx
+++ b/KMP_fault_seeded.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>description of the fault</t>
   </si>
@@ -43,7 +48,7 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -53,7 +58,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -64,7 +69,7 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -74,7 +79,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -90,7 +95,7 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -100,7 +105,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -119,7 +124,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -134,7 +139,7 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -149,7 +154,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -159,7 +164,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -174,7 +179,7 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -189,7 +194,7 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -199,7 +204,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -215,7 +220,7 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -225,7 +230,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -241,7 +246,7 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -249,32 +254,187 @@
     </r>
   </si>
   <si>
-    <t>~</t>
+    <r>
+      <t xml:space="preserve">                &amp;&amp; pattern.charAt(i) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pattern.charAt(j)) {</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      while (offset </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//&gt;=</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      if (pattern.length() &lt; MIN_LENGTH   || pattern.length() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&gt;= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MAX_LENGTH) {</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        else if (pattern.charAt(i) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pattern.charAt(j)) next[i] = j;</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        while (j </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0 //&gt;=0</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -282,7 +442,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -295,7 +461,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -318,89 +484,42 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -699,232 +818,326 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="74.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="5" t="s">
+    <row r="1" spans="1:6" ht="15">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7" t="s">
+    <row r="2" spans="1:6" ht="15">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75">
-      <c r="A3" s="4" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1">
+      <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
         <v>46</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="7">
-        <v>1</v>
-      </c>
-      <c r="F3" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75">
-      <c r="A4" s="3"/>
-      <c r="B4" s="7">
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15">
+      <c r="A4" s="11"/>
+      <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>47</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="7">
-        <v>1</v>
-      </c>
-      <c r="F4" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75">
-      <c r="A5" s="3"/>
-      <c r="B5" s="7">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15">
+      <c r="A5" s="11"/>
+      <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="1">
         <v>60</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="7">
-        <v>1</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75">
-      <c r="A6" s="3"/>
-      <c r="B6" s="7">
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15">
+      <c r="A6" s="11"/>
+      <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15">
+      <c r="A7" s="11"/>
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7">
+        <v>22</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15">
+      <c r="A8" s="11"/>
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15">
+      <c r="A9" s="11"/>
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>63</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15">
+      <c r="A10" s="11"/>
+      <c r="B10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>61</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15">
+      <c r="A11" s="11"/>
+      <c r="B11" s="1">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>61</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15">
+      <c r="A12" s="11"/>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15">
+      <c r="A13" s="11"/>
+      <c r="B13" s="7">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7">
+        <v>78</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75">
-      <c r="A7" s="3"/>
-      <c r="B7" s="7">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75">
-      <c r="A8" s="3"/>
-      <c r="B8" s="7">
-        <v>6</v>
-      </c>
-      <c r="C8" s="7">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="E13" s="6">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15">
+      <c r="A14" s="11"/>
+      <c r="B14" s="7">
         <v>12</v>
       </c>
-      <c r="E8" s="7">
-        <v>1</v>
-      </c>
-      <c r="F8" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75">
-      <c r="A9" s="3"/>
-      <c r="B9" s="7">
-        <v>7</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75">
-      <c r="A10" s="3"/>
-      <c r="B10" s="7">
-        <v>8</v>
-      </c>
-      <c r="C10" s="7">
-        <v>61</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="C14" s="7">
+        <v>75</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15">
+      <c r="A15" s="11"/>
+      <c r="B15" s="7">
         <v>13</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75">
-      <c r="A11" s="3"/>
-      <c r="B11" s="7">
-        <v>9</v>
-      </c>
-      <c r="C11" s="7">
-        <v>61</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75">
-      <c r="A12" s="2"/>
-      <c r="B12" s="7">
-        <v>10</v>
-      </c>
-      <c r="C12" s="7">
-        <v>6</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="7">
-        <v>1</v>
-      </c>
-      <c r="F12" s="7">
+      <c r="C15" s="7">
+        <v>46</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7">
+        <v>77</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6">
+      <c r="E17">
+        <f>SUM(E7:E16)/COUNT(E7:E16)</f>
+        <v>0.5</v>
+      </c>
+      <c r="F17">
+        <f>SUM(F7:F16)/COUNT(F7:F16)</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A3:A12"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:A15"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -934,9 +1147,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -946,8 +1165,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finish 20 faults in each file
</commit_message>
<xml_diff>
--- a/KMP_fault_seeded.xlsx
+++ b/KMP_fault_seeded.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>description of the fault</t>
   </si>
@@ -35,363 +35,500 @@
     <t>fault code</t>
   </si>
   <si>
+    <t>mutation test(100%)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">pattern.length() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> MIN_LENGTH || pattern.length() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> MAX_LENGTH</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">count </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (offset &gt;= 0 ? 1 : 0);</t>
+    </r>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">return </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">next[i] = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>j = next[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">return </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>text.substring(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>offset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, text.length());</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>text.substring(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>offset - 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, text.length());</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MIN_LENGTH = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                &amp;&amp; pattern.charAt(i) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pattern.charAt(j)) {</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      while (offset </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//&gt;=</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      if (pattern.length() &lt; MIN_LENGTH   || pattern.length() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&gt;= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MAX_LENGTH) {</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        else if (pattern.charAt(i) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pattern.charAt(j)) next[i] = j;</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        while (j </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0 //&gt;=0</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
     <t>Knuth Morris Pratt</t>
-  </si>
-  <si>
-    <t>mutation test(100%)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">pattern.length() </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&gt;=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> MIN_LENGTH || pattern.length() </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> MAX_LENGTH</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">count </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (offset &gt;= 0 ? 1 : 0);</t>
-    </r>
-  </si>
-  <si>
-    <t>74</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">return </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">next[i] = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>j = next[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">return </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>text.substring(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>offset</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, text.length());</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>text.substring(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>offset - 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, text.length());</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">MIN_LENGTH = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">                &amp;&amp; pattern.charAt(i) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>==</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> pattern.charAt(j)) {</t>
-    </r>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">      while (offset </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 0);</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>//&gt;=</t>
+      <t xml:space="preserve">        count += (offset &gt;= 0 ? 1 : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>);</t>
     </r>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">      if (pattern.length() &lt; MIN_LENGTH   || pattern.length() </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">&gt;= </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>MAX_LENGTH) {</t>
+      <t xml:space="preserve">        else if (pattern.charAt(i) != pattern.charAt(j)) next[i] = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>next[j];</t>
     </r>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">        else if (pattern.charAt(i) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>==</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> pattern.charAt(j)) next[i] = j;</t>
+      <t xml:space="preserve">      return </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;</t>
     </r>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">        while (j </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 0 //&gt;=0</t>
+      <t xml:space="preserve">        text = text.substring(offset </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1, text.length());</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      if (j </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>!=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pattern.length()) return i - pattern.length();</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j+=2;</t>
     </r>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -489,12 +626,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -508,14 +642,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal 2" xfId="1"/>
@@ -818,25 +956,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="74.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10"/>
+    <row r="1" spans="1:6" ht="15" customHeight="1">
+      <c r="A1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="12"/>
       <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
@@ -845,25 +985,23 @@
         <v>1</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">
-      <c r="A3" s="11" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="11"/>
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -871,7 +1009,7 @@
         <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -885,11 +1023,11 @@
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>47</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>9</v>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -907,7 +1045,7 @@
         <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -921,13 +1059,13 @@
       <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5">
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4">
         <v>1</v>
       </c>
       <c r="F6" s="1">
@@ -939,11 +1077,11 @@
       <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>22</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>11</v>
+      <c r="D7" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -961,7 +1099,7 @@
         <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -978,8 +1116,8 @@
       <c r="C9" s="1">
         <v>63</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>17</v>
+      <c r="D9" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -997,7 +1135,7 @@
         <v>61</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -1015,7 +1153,7 @@
         <v>61</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -1033,7 +1171,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -1044,91 +1182,204 @@
     </row>
     <row r="13" spans="1:6" ht="15">
       <c r="A13" s="11"/>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>11</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>78</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="6">
+      <c r="D13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="5">
         <v>0</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15">
       <c r="A14" s="11"/>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>12</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>75</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="7">
+      <c r="D14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="6">
         <v>0</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15">
       <c r="A15" s="11"/>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>13</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>46</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15">
+      <c r="A16" s="11"/>
+      <c r="B16" s="6">
+        <v>14</v>
+      </c>
+      <c r="C16" s="6">
+        <v>77</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15">
+      <c r="A17" s="11"/>
+      <c r="B17" s="6">
+        <v>15</v>
+      </c>
+      <c r="C17" s="6">
+        <v>75</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15">
+      <c r="A18" s="11"/>
+      <c r="B18" s="6">
+        <v>16</v>
+      </c>
+      <c r="C18" s="6">
+        <v>60</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15">
+      <c r="A19" s="11"/>
+      <c r="B19" s="6">
+        <v>17</v>
+      </c>
+      <c r="C19" s="6">
+        <v>61</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15">
+      <c r="A20" s="11"/>
+      <c r="B20" s="6">
         <v>18</v>
       </c>
-      <c r="E15" s="7">
-        <v>0</v>
-      </c>
-      <c r="F15" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7">
-        <v>77</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="C20" s="6">
+        <v>33</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15">
+      <c r="A21" s="11"/>
+      <c r="B21" s="6">
+        <v>19</v>
+      </c>
+      <c r="C21" s="6">
+        <v>30</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1</v>
+      </c>
+      <c r="F21" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15">
+      <c r="A22" s="11"/>
+      <c r="B22" s="6">
         <v>20</v>
       </c>
-      <c r="E16" s="7">
-        <v>0</v>
-      </c>
-      <c r="F16" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="5:6">
-      <c r="E17">
-        <f>SUM(E7:E16)/COUNT(E7:E16)</f>
-        <v>0.5</v>
-      </c>
-      <c r="F17">
-        <f>SUM(F7:F16)/COUNT(F7:F16)</f>
+      <c r="C22" s="5">
+        <v>81</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="5">
+        <v>1</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15">
+      <c r="A23" s="11"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5">
+        <f>SUM(E3:E22)/COUNT(E3:E22)</f>
+        <v>0.7</v>
+      </c>
+      <c r="F23" s="5">
+        <f>SUM(F3:F22)/COUNT(F3:F22)</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
+    <mergeCell ref="A1:A23"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="A3:A15"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>